<commit_message>
updated sim and ui
</commit_message>
<xml_diff>
--- a/Mk1 Data Sheet.xlsx
+++ b/Mk1 Data Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Desktop\python\PythonSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC97113A-D6FC-4806-B560-794AFFA074A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F37A04-4DA3-44B9-92A3-31D3DEAAD4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="795" windowWidth="16080" windowHeight="14805" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12720" yWindow="660" windowWidth="16080" windowHeight="14805" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Volume Calculations" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="73">
   <si>
     <t>Supposed More Accurate Equations for Rocket Motion</t>
   </si>
@@ -143,9 +143,6 @@
   </si>
   <si>
     <t>Mass Struct:</t>
-  </si>
-  <si>
-    <t>Payload Mass:</t>
   </si>
   <si>
     <t>Total Initial Mass</t>
@@ -605,6 +602,33 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -621,33 +645,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1075,23 +1072,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="10"/>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="47"/>
+      <c r="B2" s="56"/>
       <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>21</v>
@@ -1099,7 +1096,7 @@
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="16">
         <v>12</v>
@@ -1128,35 +1125,35 @@
     </row>
     <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="38">
         <f>PI()*(C4/2)^2*(C5/3)</f>
         <v>1.4826755164729137E-2</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="58"/>
+      <c r="C9" s="21"/>
+    </row>
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="49"/>
-      <c r="C9" s="21"/>
-    </row>
-    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="51"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="22"/>
     </row>
     <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23"/>
       <c r="B11" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>21</v>
@@ -1164,7 +1161,7 @@
     </row>
     <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="25">
         <f>C12*39.37</f>
@@ -1176,7 +1173,7 @@
     </row>
     <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="25">
         <f>C13*39.37</f>
@@ -1188,7 +1185,7 @@
     </row>
     <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="25">
         <f>C14*39.37</f>
@@ -1205,30 +1202,30 @@
     </row>
     <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="39">
         <f>(1/3)*PI()*C14*(C12^2+C13^2+(C12*C13))</f>
         <v>1.0070336348177904E-2</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="49"/>
+      <c r="B18" s="58"/>
       <c r="C18" s="29"/>
       <c r="D18" s="30"/>
     </row>
     <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="51"/>
+      <c r="A19" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="46"/>
       <c r="C19" s="31"/>
       <c r="D19" s="32"/>
     </row>
@@ -1242,7 +1239,7 @@
     </row>
     <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="33">
         <v>2.9000000000000001E-2</v>
@@ -1261,82 +1258,82 @@
       <c r="D22" s="32"/>
     </row>
     <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="53" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="54"/>
+      <c r="A23" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="48"/>
       <c r="C23" s="31"/>
       <c r="D23" s="32"/>
     </row>
     <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="37">
         <f>PI()*(B21/2)^2*B22</f>
         <v>7.5299263517566965E-5</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="32"/>
     </row>
     <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="55" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="56"/>
+      <c r="A25" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="50"/>
       <c r="C25" s="40">
         <f>B24*30</f>
         <v>2.258977905527009E-3</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="57" t="s">
+      <c r="A27" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="52"/>
+      <c r="D27" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="58"/>
-      <c r="D27" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="57"/>
+      <c r="E27" s="51"/>
     </row>
     <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="52">
+      <c r="D28" s="44">
         <v>0.6</v>
       </c>
-      <c r="E28" s="52"/>
+      <c r="E28" s="44"/>
     </row>
     <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="8">
         <f>B7-B16-C25</f>
         <v>2.497440911024224E-3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D29" s="35">
         <f>B29*(D28+0.15)</f>
         <v>1.873080683268168E-3</v>
       </c>
       <c r="E29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" t="s">
         <v>63</v>
-      </c>
-      <c r="E31" t="s">
-        <v>64</v>
       </c>
       <c r="F31" s="4">
         <v>1100</v>
@@ -1348,7 +1345,7 @@
     <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B33" s="35">
         <f>D29*F31</f>
@@ -1360,17 +1357,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A18:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1384,7 +1381,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,13 +1398,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="51" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="59"/>
     </row>
     <row r="2" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="59"/>
@@ -1417,12 +1414,12 @@
       <c r="D2" s="8">
         <v>30</v>
       </c>
-      <c r="F2" s="57" t="s">
-        <v>66</v>
+      <c r="F2" s="51" t="s">
+        <v>65</v>
       </c>
       <c r="G2" s="59"/>
-      <c r="J2" s="57" t="s">
-        <v>73</v>
+      <c r="J2" s="51" t="s">
+        <v>72</v>
       </c>
       <c r="K2" s="59"/>
     </row>
@@ -1616,7 +1613,7 @@
     </row>
     <row r="11" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="9">
         <v>4.5699999999999998E-2</v>
@@ -1625,7 +1622,7 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G11" s="9">
         <v>4.2000000000000003E-2</v>
@@ -1634,7 +1631,7 @@
         <v>15</v>
       </c>
       <c r="J11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K11" s="9">
         <v>8.6999999999999994E-2</v>
@@ -1645,7 +1642,7 @@
     </row>
     <row r="12" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="9">
         <v>2.4199999999999999E-2</v>
@@ -1654,7 +1651,7 @@
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G12" s="9">
         <v>0.06</v>
@@ -1663,7 +1660,7 @@
         <v>15</v>
       </c>
       <c r="J12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K12" s="9">
         <v>0.1164</v>
@@ -1674,7 +1671,7 @@
     </row>
     <row r="13" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="9">
         <f>B12+B11</f>
@@ -1684,7 +1681,7 @@
         <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G13" s="9">
         <f>G12+G11</f>
@@ -1694,7 +1691,7 @@
         <v>15</v>
       </c>
       <c r="J13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K13" s="9">
         <v>0.2034</v>
@@ -1705,7 +1702,7 @@
     </row>
     <row r="14" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="43">
         <f>(B11+B12)*$D$2</f>
@@ -1715,7 +1712,7 @@
         <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G14" s="43">
         <f>(G11+G12)*$D$2</f>
@@ -1725,7 +1722,7 @@
         <v>15</v>
       </c>
       <c r="J14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K14" s="43">
         <v>6.1020000000000003</v>
@@ -1736,7 +1733,7 @@
     </row>
     <row r="15" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" s="1">
         <f>B12*$D$2</f>
@@ -1746,7 +1743,7 @@
         <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G15" s="1">
         <f>G12*$D$2</f>
@@ -1756,7 +1753,7 @@
         <v>15</v>
       </c>
       <c r="J15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K15" s="1">
         <v>3.492</v>
@@ -1767,7 +1764,7 @@
     </row>
     <row r="16" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" s="9">
         <f>B11-B12+B20</f>
@@ -1777,7 +1774,7 @@
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G16" s="9">
         <f>G11-G12+G20</f>
@@ -1787,7 +1784,7 @@
         <v>15</v>
       </c>
       <c r="J16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K16" s="9">
         <v>2.0309887515949852</v>
@@ -1916,33 +1913,12 @@
       <c r="L21" s="7"/>
     </row>
     <row r="22" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="9">
-        <v>0</v>
-      </c>
-      <c r="C22" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" s="9">
-        <v>0</v>
-      </c>
-      <c r="H22" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="J22" t="s">
-        <v>36</v>
-      </c>
-      <c r="K22" s="9">
-        <v>0</v>
-      </c>
-      <c r="L22" s="41" t="s">
-        <v>15</v>
-      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="41"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="41"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="41"/>
     </row>
     <row r="23" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
@@ -1954,7 +1930,7 @@
     </row>
     <row r="24" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="9">
         <f>B14+B20+B22</f>
@@ -1964,7 +1940,7 @@
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G24" s="9">
         <f>G22+G20+G14</f>
@@ -1974,7 +1950,7 @@
         <v>15</v>
       </c>
       <c r="J24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K24" s="9">
         <v>8.1623887515949853</v>
@@ -1989,7 +1965,7 @@
     </row>
     <row r="26" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="9">
         <f>B9/(B20*9.8+B11*9.8+B22*9.8)</f>
@@ -2003,31 +1979,31 @@
     </row>
     <row r="28" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" s="9">
         <v>20</v>
       </c>
       <c r="C28" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G28" s="9">
         <v>49.61</v>
       </c>
       <c r="H28" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K28" s="9">
         <v>211.2</v>
       </c>
       <c r="L28" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2036,7 +2012,7 @@
     </row>
     <row r="30" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" s="9">
         <f>B28/(9.81*B12)</f>
@@ -2046,14 +2022,14 @@
         <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G30" s="9">
         <f>G28/(9.81*G12)</f>
         <v>84.284743459055377</v>
       </c>
       <c r="J30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K30" s="9">
         <f>K28/(9.81*K12)</f>
@@ -2066,7 +2042,7 @@
     </row>
     <row r="32" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32" s="9">
         <f>(9.81)*(B30)*LN((B24)/(B24-B12))</f>
@@ -2082,7 +2058,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="9">
         <v>343</v>
@@ -2097,7 +2073,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="9">
         <f>B32/B34</f>

</xml_diff>